<commit_message>
1. fixed strore_results(), t_test() and all_results_colorful() 2. fixed all_datasets_results.csv, all_resualts_colors.xlsx & t_test_results.csv
</commit_message>
<xml_diff>
--- a/results/all_resualts_colors.xlsx
+++ b/results/all_resualts_colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omerh\PycharmProjects\Thesis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A342FC-C93D-4A31-A67D-4067C305F88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6544EBF-723E-490B-9F13-EC53ECE3D6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="390" windowWidth="28770" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>